<commit_message>
Production of processing StudySettings
</commit_message>
<xml_diff>
--- a/tests/test_files/Inputs.xlsx
+++ b/tests/test_files/Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA93921-5381-4575-94A6-50AE0CD406E4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4BF04C-FDF0-4DB4-B047-A0BAE639F2C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="2070" windowWidth="21600" windowHeight="11385" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4095" yWindow="3015" windowWidth="21585" windowHeight="11385" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -1087,9 +1087,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>EirGrid.ElmNet</t>
-  </si>
-  <si>
     <t>220 kV A1</t>
   </si>
   <si>
@@ -1224,6 +1221,9 @@
   </si>
   <si>
     <t>Export_to_Excel</t>
+  </si>
+  <si>
+    <t>NSW.ElmNet</t>
   </si>
 </sst>
 </file>
@@ -1593,6 +1593,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1617,7 +1618,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2011,7 +2011,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2021,7 +2021,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2043,7 +2043,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C7" s="4">
         <v>43954</v>
@@ -2085,7 +2085,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2102,14 +2102,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
-        <v>257</v>
+      <c r="A2" s="40" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
@@ -2118,32 +2118,32 @@
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>221</v>
+        <v>262</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>219</v>
@@ -2173,13 +2173,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B10" s="22" t="b">
         <v>1</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2208,7 +2208,7 @@
   <mergeCells count="1">
     <mergeCell ref="D3:F3"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B12" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"True,False"</formula1>
     </dataValidation>
@@ -2260,16 +2260,16 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="34" t="s">
         <v>240</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="C5" s="34" t="s">
         <v>241</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="D5" s="34" t="s">
         <v>242</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2409,51 +2409,51 @@
     </row>
     <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="41" t="s">
+      <c r="C3" s="46"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="41" t="s">
+      <c r="F3" s="43"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="41" t="s">
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="42"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="41" t="s">
+      <c r="L3" s="43"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="42"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="41" t="s">
+      <c r="O3" s="43"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="42"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="41" t="s">
+      <c r="R3" s="43"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="U3" s="42"/>
-      <c r="V3" s="43"/>
-      <c r="W3" s="41" t="s">
+      <c r="U3" s="43"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="X3" s="42"/>
-      <c r="Y3" s="43"/>
-      <c r="Z3" s="41" t="s">
+      <c r="X3" s="43"/>
+      <c r="Y3" s="44"/>
+      <c r="Z3" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="AA3" s="42"/>
-      <c r="AB3" s="43"/>
+      <c r="AA3" s="43"/>
+      <c r="AB3" s="44"/>
     </row>
     <row r="4" spans="1:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
@@ -2543,7 +2543,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -6046,18 +6046,18 @@
         <v>20</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D5" s="3" t="b">
         <v>0</v>
@@ -6065,13 +6065,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D6" s="3" t="b">
         <v>0</v>
@@ -6697,17 +6697,17 @@
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>18</v>
@@ -6716,31 +6716,31 @@
         <v>20</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E4" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="F4" s="36" t="s">
         <v>229</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="G4" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="H4" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="G4" s="36" t="s">
-        <v>235</v>
-      </c>
-      <c r="H4" s="36" t="s">
+      <c r="I4" s="36" t="s">
         <v>231</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="J4" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="K4" s="36" t="s">
         <v>232</v>
       </c>
-      <c r="J4" s="36" t="s">
-        <v>235</v>
-      </c>
-      <c r="K4" s="36" t="s">
+      <c r="L4" s="36" t="s">
         <v>233</v>
-      </c>
-      <c r="L4" s="36" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -8175,16 +8175,16 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
+        <v>249</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4" t="s">
         <v>250</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="E4" s="1" t="str">
         <f>IF($D$4="","&lt;--- Cannot be empty, please enter False","")</f>
@@ -8194,7 +8194,7 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="48" t="s">
         <v>136</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -8208,7 +8208,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
+      <c r="A6" s="48"/>
       <c r="B6" s="12" t="s">
         <v>82</v>
       </c>
@@ -8220,7 +8220,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="12" t="s">
         <v>91</v>
       </c>
@@ -8232,19 +8232,19 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="C8" t="s">
         <v>248</v>
-      </c>
-      <c r="C8" t="s">
-        <v>249</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
+      <c r="A9" s="48"/>
       <c r="B9" s="12" t="s">
         <v>83</v>
       </c>
@@ -8256,7 +8256,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
+      <c r="A10" s="48"/>
       <c r="B10" s="12" t="s">
         <v>84</v>
       </c>
@@ -8268,7 +8268,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
+      <c r="A11" s="48"/>
       <c r="B11" s="12" t="s">
         <v>92</v>
       </c>
@@ -8280,7 +8280,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="12" t="s">
         <v>85</v>
       </c>
@@ -8292,7 +8292,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="12" t="s">
         <v>86</v>
       </c>
@@ -8304,7 +8304,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="12" t="s">
         <v>87</v>
       </c>
@@ -8316,7 +8316,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
+      <c r="A15" s="48"/>
       <c r="B15" s="12" t="s">
         <v>88</v>
       </c>
@@ -8328,7 +8328,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="48" t="s">
         <v>137</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -8342,7 +8342,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
+      <c r="A17" s="48"/>
       <c r="B17" s="12" t="s">
         <v>93</v>
       </c>
@@ -8354,7 +8354,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="48"/>
       <c r="B18" s="12" t="s">
         <v>94</v>
       </c>
@@ -8366,19 +8366,19 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+      <c r="A19" s="48"/>
       <c r="B19" s="16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>144</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="12" t="s">
         <v>95</v>
       </c>
@@ -8390,7 +8390,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="48" t="s">
         <v>138</v>
       </c>
       <c r="B21" s="12" t="s">
@@ -8404,7 +8404,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="12" t="s">
         <v>97</v>
       </c>
@@ -8416,7 +8416,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
+      <c r="A23" s="48"/>
       <c r="B23" s="12" t="s">
         <v>98</v>
       </c>
@@ -8428,7 +8428,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
+      <c r="A24" s="48"/>
       <c r="B24" s="12" t="s">
         <v>99</v>
       </c>
@@ -8440,7 +8440,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
+      <c r="A25" s="48"/>
       <c r="B25" s="12" t="s">
         <v>100</v>
       </c>
@@ -8452,7 +8452,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
+      <c r="A26" s="48"/>
       <c r="B26" s="12" t="s">
         <v>101</v>
       </c>
@@ -8464,7 +8464,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
+      <c r="A27" s="48"/>
       <c r="B27" s="12" t="s">
         <v>102</v>
       </c>
@@ -8476,7 +8476,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
+      <c r="A28" s="48"/>
       <c r="B28" s="12" t="s">
         <v>103</v>
       </c>
@@ -8488,7 +8488,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
+      <c r="A29" s="48"/>
       <c r="B29" s="12" t="s">
         <v>104</v>
       </c>
@@ -8500,7 +8500,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
+      <c r="A30" s="48"/>
       <c r="B30" s="12" t="s">
         <v>105</v>
       </c>
@@ -8512,7 +8512,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
+      <c r="A31" s="48"/>
       <c r="B31" s="12" t="s">
         <v>106</v>
       </c>
@@ -8524,7 +8524,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="48" t="s">
         <v>139</v>
       </c>
       <c r="B32" s="12" t="s">
@@ -8538,7 +8538,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
+      <c r="A33" s="48"/>
       <c r="B33" s="12" t="s">
         <v>108</v>
       </c>
@@ -8550,7 +8550,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="47"/>
+      <c r="A34" s="48"/>
       <c r="B34" s="12" t="s">
         <v>109</v>
       </c>
@@ -8562,7 +8562,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
+      <c r="A35" s="48"/>
       <c r="B35" s="12" t="s">
         <v>110</v>
       </c>
@@ -8574,7 +8574,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
+      <c r="A36" s="48"/>
       <c r="B36" s="12" t="s">
         <v>111</v>
       </c>
@@ -8586,7 +8586,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="47"/>
+      <c r="A37" s="48"/>
       <c r="B37" s="12" t="s">
         <v>112</v>
       </c>
@@ -8598,7 +8598,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="47"/>
+      <c r="A38" s="48"/>
       <c r="B38" s="12" t="s">
         <v>113</v>
       </c>
@@ -8610,7 +8610,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="47"/>
+      <c r="A39" s="48"/>
       <c r="B39" s="12" t="s">
         <v>114</v>
       </c>
@@ -8622,7 +8622,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="47" t="s">
+      <c r="A40" s="48" t="s">
         <v>140</v>
       </c>
       <c r="B40" s="12" t="s">
@@ -8636,7 +8636,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="47"/>
+      <c r="A41" s="48"/>
       <c r="B41" s="12" t="s">
         <v>116</v>
       </c>
@@ -8648,7 +8648,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="47"/>
+      <c r="A42" s="48"/>
       <c r="B42" s="12" t="s">
         <v>117</v>
       </c>
@@ -8660,7 +8660,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="47"/>
+      <c r="A43" s="48"/>
       <c r="B43" s="12" t="s">
         <v>118</v>
       </c>
@@ -8672,7 +8672,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="47"/>
+      <c r="A44" s="48"/>
       <c r="B44" s="12" t="s">
         <v>119</v>
       </c>
@@ -8684,7 +8684,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="47"/>
+      <c r="A45" s="48"/>
       <c r="B45" s="12" t="s">
         <v>120</v>
       </c>
@@ -8696,7 +8696,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="47"/>
+      <c r="A46" s="48"/>
       <c r="B46" s="12" t="s">
         <v>121</v>
       </c>
@@ -8708,7 +8708,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="47"/>
+      <c r="A47" s="48"/>
       <c r="B47" s="16" t="s">
         <v>122</v>
       </c>
@@ -8720,7 +8720,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="47"/>
+      <c r="A48" s="48"/>
       <c r="B48" s="12" t="s">
         <v>123</v>
       </c>
@@ -8732,7 +8732,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="47"/>
+      <c r="A49" s="48"/>
       <c r="B49" s="16" t="s">
         <v>124</v>
       </c>
@@ -8744,7 +8744,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="47" t="s">
+      <c r="A50" s="48" t="s">
         <v>141</v>
       </c>
       <c r="B50" s="12" t="s">
@@ -8758,7 +8758,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="47"/>
+      <c r="A51" s="48"/>
       <c r="B51" s="12" t="s">
         <v>126</v>
       </c>
@@ -8770,7 +8770,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="47"/>
+      <c r="A52" s="48"/>
       <c r="B52" s="12" t="s">
         <v>127</v>
       </c>
@@ -8782,7 +8782,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="47" t="s">
+      <c r="A53" s="48" t="s">
         <v>142</v>
       </c>
       <c r="B53" s="12" t="s">
@@ -8796,7 +8796,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="47"/>
+      <c r="A54" s="48"/>
       <c r="B54" s="12" t="s">
         <v>129</v>
       </c>
@@ -8808,7 +8808,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="47"/>
+      <c r="A55" s="48"/>
       <c r="B55" s="12" t="s">
         <v>130</v>
       </c>
@@ -8820,7 +8820,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="47"/>
+      <c r="A56" s="48"/>
       <c r="B56" s="12" t="s">
         <v>131</v>
       </c>
@@ -8832,7 +8832,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="47"/>
+      <c r="A57" s="48"/>
       <c r="B57" s="12" t="s">
         <v>132</v>
       </c>
@@ -8844,7 +8844,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="47"/>
+      <c r="A58" s="48"/>
       <c r="B58" s="12" t="s">
         <v>133</v>
       </c>
@@ -8856,7 +8856,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="47" t="s">
+      <c r="A59" s="48" t="s">
         <v>143</v>
       </c>
       <c r="B59" s="12" t="s">
@@ -8870,7 +8870,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="47"/>
+      <c r="A60" s="48"/>
       <c r="B60" s="12" t="s">
         <v>135</v>
       </c>
@@ -8951,7 +8951,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="48" t="s">
         <v>146</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -8965,7 +8965,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
+      <c r="A6" s="48"/>
       <c r="B6" s="12" t="s">
         <v>183</v>
       </c>
@@ -8977,7 +8977,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="12" t="s">
         <v>184</v>
       </c>
@@ -8989,7 +8989,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="12" t="s">
         <v>185</v>
       </c>
@@ -9001,7 +9001,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
+      <c r="A9" s="48"/>
       <c r="B9" s="12" t="s">
         <v>186</v>
       </c>
@@ -9014,7 +9014,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
+      <c r="A10" s="48"/>
       <c r="B10" s="12" t="s">
         <v>187</v>
       </c>
@@ -9026,7 +9026,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
+      <c r="A11" s="48"/>
       <c r="B11" s="12" t="s">
         <v>188</v>
       </c>
@@ -9038,7 +9038,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="12" t="s">
         <v>182</v>
       </c>
@@ -9051,7 +9051,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="12" t="s">
         <v>189</v>
       </c>
@@ -9064,7 +9064,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="12" t="s">
         <v>190</v>
       </c>
@@ -9077,7 +9077,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
+      <c r="A15" s="48"/>
       <c r="B15" s="16" t="s">
         <v>191</v>
       </c>
@@ -9089,7 +9089,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="16" t="s">
         <v>192</v>
       </c>
@@ -9101,7 +9101,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="48" t="s">
         <v>147</v>
       </c>
       <c r="B17" s="12" t="s">
@@ -9115,7 +9115,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="48"/>
       <c r="B18" s="12" t="s">
         <v>194</v>
       </c>
@@ -9127,7 +9127,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+      <c r="A19" s="48"/>
       <c r="B19" s="12" t="s">
         <v>195</v>
       </c>
@@ -9139,7 +9139,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="12" t="s">
         <v>196</v>
       </c>
@@ -9184,12 +9184,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B1" s="7"/>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
+      <c r="A5" s="48"/>
       <c r="B5" s="12" t="s">
         <v>218</v>
       </c>
@@ -9201,7 +9201,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
+      <c r="A6" s="48"/>
       <c r="B6" s="12" t="s">
         <v>197</v>
       </c>
@@ -9213,7 +9213,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="12" t="s">
         <v>198</v>
       </c>
@@ -9225,7 +9225,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="12" t="s">
         <v>199</v>
       </c>
@@ -9237,7 +9237,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
+      <c r="A9" s="48"/>
       <c r="B9" s="12" t="s">
         <v>182</v>
       </c>
@@ -9249,7 +9249,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
+      <c r="A10" s="48"/>
       <c r="B10" s="12" t="s">
         <v>189</v>
       </c>
@@ -9261,7 +9261,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
+      <c r="A11" s="48"/>
       <c r="B11" s="12" t="s">
         <v>190</v>
       </c>
@@ -9274,7 +9274,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="16" t="s">
         <v>191</v>
       </c>
@@ -9286,7 +9286,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="16" t="s">
         <v>192</v>
       </c>
@@ -9312,7 +9312,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="48" t="s">
         <v>180</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -9326,7 +9326,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="12" t="s">
         <v>202</v>
       </c>
@@ -9338,7 +9338,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
+      <c r="A17" s="48"/>
       <c r="B17" s="12" t="s">
         <v>203</v>
       </c>
@@ -9350,7 +9350,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="48"/>
       <c r="B18" s="12" t="s">
         <v>196</v>
       </c>
@@ -9362,7 +9362,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+      <c r="A19" s="48"/>
       <c r="B19" s="12" t="s">
         <v>204</v>
       </c>
@@ -9388,26 +9388,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </iab7cdb7554d4997ae876b11632fa575>
-    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -9559,31 +9539,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </iab7cdb7554d4997ae876b11632fa575>
+    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9599,4 +9575,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Processing of StudyCases into suitable format completed
</commit_message>
<xml_diff>
--- a/tests/test_files/Inputs.xlsx
+++ b/tests/test_files/Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4BF04C-FDF0-4DB4-B047-A0BAE639F2C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FE37A8-7D67-47B2-9867-1D6B26B0A89C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="3015" windowWidth="21585" windowHeight="11385" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4095" yWindow="3015" windowWidth="21585" windowHeight="11385" tabRatio="868" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -422,7 +422,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="263">
   <si>
     <t>Name</t>
   </si>
@@ -2084,7 +2084,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2223,8 +2223,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,10 +2273,18 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
+      <c r="A6" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -9388,6 +9396,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </iab7cdb7554d4997ae876b11632fa575>
+    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -9539,27 +9567,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </iab7cdb7554d4997ae876b11632fa575>
-    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9575,28 +9607,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating processing of input data
</commit_message>
<xml_diff>
--- a/tests/test_files/Inputs.xlsx
+++ b/tests/test_files/Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FE37A8-7D67-47B2-9867-1D6B26B0A89C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B599E7A-6A43-4D91-91FA-34518B60499F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="3015" windowWidth="21585" windowHeight="11385" tabRatio="868" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4095" yWindow="3015" windowWidth="21585" windowHeight="11385" tabRatio="868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -422,7 +422,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="263">
   <si>
     <t>Name</t>
   </si>
@@ -2223,7 +2223,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2394,8 +2394,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AB165"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2584,8 +2584,12 @@
       <c r="AB5" s="3"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -8156,7 +8160,7 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9396,26 +9400,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </iab7cdb7554d4997ae876b11632fa575>
-    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -9567,31 +9551,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </iab7cdb7554d4997ae876b11632fa575>
+    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9607,4 +9587,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated file_io to include processing of load flow settings
</commit_message>
<xml_diff>
--- a/tests/test_files/Inputs.xlsx
+++ b/tests/test_files/Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B599E7A-6A43-4D91-91FA-34518B60499F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251A8BC9-0CF5-4A85-B965-21B5DF0620B9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="3015" windowWidth="21585" windowHeight="11385" tabRatio="868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30120" yWindow="2610" windowWidth="21600" windowHeight="11385" tabRatio="868" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -1157,15 +1157,6 @@
     <t>BASE</t>
   </si>
   <si>
-    <t>AIM 2019-MODEL-RELEASE v1.0(JI7867)</t>
-  </si>
-  <si>
-    <t>CP966</t>
-  </si>
-  <si>
-    <t>SV-HW</t>
-  </si>
-  <si>
     <t>EirGrid\Turlough Hill\220 kV T2001/2 TCB</t>
   </si>
   <si>
@@ -1224,6 +1215,15 @@
   </si>
   <si>
     <t>NSW.ElmNet</t>
+  </si>
+  <si>
+    <t>High Load Case</t>
+  </si>
+  <si>
+    <t>HighLoadTap_testing</t>
+  </si>
+  <si>
+    <t>pscharmonics_test_model</t>
   </si>
 </sst>
 </file>
@@ -2011,7 +2011,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2021,7 +2021,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2103,7 +2103,7 @@
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="40" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2118,32 +2118,32 @@
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>236</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>219</v>
@@ -2173,7 +2173,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B10" s="22" t="b">
         <v>1</v>
@@ -2223,7 +2223,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2263,13 +2263,13 @@
         <v>239</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>240</v>
+        <v>262</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>241</v>
+        <v>260</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2277,13 +2277,13 @@
         <v>239</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>240</v>
+        <v>262</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>241</v>
+        <v>260</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2394,7 +2394,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AB165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -6063,10 +6063,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>221</v>
@@ -6077,10 +6077,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>221</v>
@@ -8187,16 +8187,16 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>252</v>
-      </c>
       <c r="C4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E4" s="1" t="str">
         <f>IF($D$4="","&lt;--- Cannot be empty, please enter False","")</f>
@@ -8246,10 +8246,10 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="48"/>
       <c r="B8" s="12" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -8380,13 +8380,13 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="48"/>
       <c r="B19" s="16" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>144</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -9400,6 +9400,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </iab7cdb7554d4997ae876b11632fa575>
+    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -9551,27 +9571,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </iab7cdb7554d4997ae876b11632fa575>
-    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9587,28 +9611,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implementation of algorithm to determine fault cases
</commit_message>
<xml_diff>
--- a/tests/test_files/Inputs.xlsx
+++ b/tests/test_files/Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72CE4E7-2AB4-4AB2-B08D-E39E60B95CDE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD719B77-35DA-4471-98FE-A68C5833616F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="2310" windowWidth="21600" windowHeight="11385" tabRatio="868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -353,7 +353,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="225">
   <si>
     <t>Name</t>
   </si>
@@ -1010,6 +1010,24 @@
   </si>
   <si>
     <t>Name of existing contingency analysis command that includes details of all of the contingencies to be considered (Set to FALSE if not using)</t>
+  </si>
+  <si>
+    <t>TEST Cont</t>
+  </si>
+  <si>
+    <t>ALBURY 132KV</t>
+  </si>
+  <si>
+    <t>Switch_213211</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>LADBROKE GROVE 132KV</t>
+  </si>
+  <si>
+    <t>Switch_210309</t>
   </si>
 </sst>
 </file>
@@ -1381,6 +1399,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1405,65 +1429,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -1514,6 +1486,23 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1963,9 +1952,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
@@ -2251,7 +2240,7 @@
   <dimension ref="A1:AB166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,143 +2273,143 @@
       <c r="C3" t="s">
         <v>217</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>216</v>
+      <c r="D3" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="30" t="s">
         <v>215</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="31" t="s">
+      <c r="C4" s="41"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="31" t="s">
+      <c r="F4" s="38"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="31" t="s">
+      <c r="I4" s="38"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="32"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="31" t="s">
+      <c r="L4" s="38"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="32"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="31" t="s">
+      <c r="O4" s="38"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="R4" s="32"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="31" t="s">
+      <c r="R4" s="38"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="U4" s="32"/>
-      <c r="V4" s="33"/>
-      <c r="W4" s="31" t="s">
+      <c r="U4" s="38"/>
+      <c r="V4" s="39"/>
+      <c r="W4" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="X4" s="32"/>
-      <c r="Y4" s="33"/>
-      <c r="Z4" s="31" t="s">
+      <c r="X4" s="38"/>
+      <c r="Y4" s="39"/>
+      <c r="Z4" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="AA4" s="32"/>
-      <c r="AB4" s="33"/>
+      <c r="AA4" s="38"/>
+      <c r="AB4" s="39"/>
     </row>
     <row r="5" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="F5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="42" t="s">
+      <c r="J5" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="K5" s="43" t="s">
+      <c r="K5" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="42" t="s">
+      <c r="L5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="42" t="s">
+      <c r="M5" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="N5" s="43" t="s">
+      <c r="N5" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="O5" s="42" t="s">
+      <c r="O5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="42" t="s">
+      <c r="P5" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="Q5" s="43" t="s">
+      <c r="Q5" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="R5" s="42" t="s">
+      <c r="R5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="S5" s="42" t="s">
+      <c r="S5" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="T5" s="43" t="s">
+      <c r="T5" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="U5" s="42" t="s">
+      <c r="U5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="V5" s="42" t="s">
+      <c r="V5" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="W5" s="43" t="s">
+      <c r="W5" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="X5" s="42" t="s">
+      <c r="X5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="Y5" s="42" t="s">
+      <c r="Y5" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="Z5" s="43" t="s">
+      <c r="Z5" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="AA5" s="42" t="s">
+      <c r="AA5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="AB5" s="42" t="s">
+      <c r="AB5" s="34" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2460,16 +2449,26 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+        <v>219</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>222</v>
+      </c>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
@@ -7279,17 +7278,17 @@
     <mergeCell ref="T4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:D3">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>$D$3=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>$D$3=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:AB166">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$D$3&lt;&gt;FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7962,12 +7961,12 @@
     <sortCondition ref="A5:A8"/>
   </sortState>
   <conditionalFormatting sqref="A5:A103">
-    <cfRule type="expression" dxfId="15" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>LEN(A5)&gt;19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>A3="NAMES OKAY"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8029,7 +8028,7 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="43" t="s">
         <v>135</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -8043,7 +8042,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
+      <c r="A6" s="43"/>
       <c r="B6" s="6" t="s">
         <v>82</v>
       </c>
@@ -8055,7 +8054,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="6" t="s">
         <v>90</v>
       </c>
@@ -8067,7 +8066,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="6" t="s">
         <v>191</v>
       </c>
@@ -8079,7 +8078,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="6" t="s">
         <v>83</v>
       </c>
@@ -8091,7 +8090,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="6" t="s">
         <v>84</v>
       </c>
@@ -8103,7 +8102,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="6" t="s">
         <v>91</v>
       </c>
@@ -8115,7 +8114,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="6" t="s">
         <v>85</v>
       </c>
@@ -8127,7 +8126,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="6" t="s">
         <v>86</v>
       </c>
@@ -8139,7 +8138,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="6" t="s">
         <v>87</v>
       </c>
@@ -8151,7 +8150,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="6" t="s">
         <v>88</v>
       </c>
@@ -8163,7 +8162,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="43" t="s">
         <v>136</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -8177,7 +8176,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="6" t="s">
         <v>92</v>
       </c>
@@ -8189,7 +8188,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="6" t="s">
         <v>93</v>
       </c>
@@ -8201,7 +8200,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="37"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="9" t="s">
         <v>188</v>
       </c>
@@ -8213,7 +8212,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="37"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="6" t="s">
         <v>94</v>
       </c>
@@ -8225,7 +8224,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="43" t="s">
         <v>137</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -8239,7 +8238,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="6" t="s">
         <v>96</v>
       </c>
@@ -8251,7 +8250,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="37"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="6" t="s">
         <v>97</v>
       </c>
@@ -8263,7 +8262,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="37"/>
+      <c r="A24" s="43"/>
       <c r="B24" s="6" t="s">
         <v>98</v>
       </c>
@@ -8275,7 +8274,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="37"/>
+      <c r="A25" s="43"/>
       <c r="B25" s="6" t="s">
         <v>99</v>
       </c>
@@ -8287,7 +8286,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="37"/>
+      <c r="A26" s="43"/>
       <c r="B26" s="6" t="s">
         <v>100</v>
       </c>
@@ -8299,7 +8298,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="37"/>
+      <c r="A27" s="43"/>
       <c r="B27" s="6" t="s">
         <v>101</v>
       </c>
@@ -8311,7 +8310,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="37"/>
+      <c r="A28" s="43"/>
       <c r="B28" s="6" t="s">
         <v>102</v>
       </c>
@@ -8323,7 +8322,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="37"/>
+      <c r="A29" s="43"/>
       <c r="B29" s="6" t="s">
         <v>103</v>
       </c>
@@ -8335,7 +8334,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="37"/>
+      <c r="A30" s="43"/>
       <c r="B30" s="6" t="s">
         <v>104</v>
       </c>
@@ -8347,7 +8346,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
+      <c r="A31" s="43"/>
       <c r="B31" s="6" t="s">
         <v>105</v>
       </c>
@@ -8359,7 +8358,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="43" t="s">
         <v>138</v>
       </c>
       <c r="B32" s="6" t="s">
@@ -8373,7 +8372,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
+      <c r="A33" s="43"/>
       <c r="B33" s="6" t="s">
         <v>107</v>
       </c>
@@ -8385,7 +8384,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="37"/>
+      <c r="A34" s="43"/>
       <c r="B34" s="6" t="s">
         <v>108</v>
       </c>
@@ -8397,7 +8396,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="37"/>
+      <c r="A35" s="43"/>
       <c r="B35" s="6" t="s">
         <v>109</v>
       </c>
@@ -8409,7 +8408,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="37"/>
+      <c r="A36" s="43"/>
       <c r="B36" s="6" t="s">
         <v>110</v>
       </c>
@@ -8421,7 +8420,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="37"/>
+      <c r="A37" s="43"/>
       <c r="B37" s="6" t="s">
         <v>111</v>
       </c>
@@ -8433,7 +8432,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="37"/>
+      <c r="A38" s="43"/>
       <c r="B38" s="6" t="s">
         <v>112</v>
       </c>
@@ -8445,7 +8444,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="37"/>
+      <c r="A39" s="43"/>
       <c r="B39" s="6" t="s">
         <v>113</v>
       </c>
@@ -8457,7 +8456,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="37" t="s">
+      <c r="A40" s="43" t="s">
         <v>139</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -8471,7 +8470,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="37"/>
+      <c r="A41" s="43"/>
       <c r="B41" s="6" t="s">
         <v>115</v>
       </c>
@@ -8483,7 +8482,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="37"/>
+      <c r="A42" s="43"/>
       <c r="B42" s="6" t="s">
         <v>116</v>
       </c>
@@ -8495,7 +8494,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="37"/>
+      <c r="A43" s="43"/>
       <c r="B43" s="6" t="s">
         <v>117</v>
       </c>
@@ -8507,7 +8506,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="37"/>
+      <c r="A44" s="43"/>
       <c r="B44" s="6" t="s">
         <v>118</v>
       </c>
@@ -8519,7 +8518,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="37"/>
+      <c r="A45" s="43"/>
       <c r="B45" s="6" t="s">
         <v>119</v>
       </c>
@@ -8531,7 +8530,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="37"/>
+      <c r="A46" s="43"/>
       <c r="B46" s="6" t="s">
         <v>120</v>
       </c>
@@ -8543,7 +8542,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="37"/>
+      <c r="A47" s="43"/>
       <c r="B47" s="9" t="s">
         <v>121</v>
       </c>
@@ -8555,7 +8554,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="37"/>
+      <c r="A48" s="43"/>
       <c r="B48" s="6" t="s">
         <v>122</v>
       </c>
@@ -8567,7 +8566,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="37"/>
+      <c r="A49" s="43"/>
       <c r="B49" s="9" t="s">
         <v>123</v>
       </c>
@@ -8579,7 +8578,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="43" t="s">
         <v>140</v>
       </c>
       <c r="B50" s="6" t="s">
@@ -8593,7 +8592,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="37"/>
+      <c r="A51" s="43"/>
       <c r="B51" s="6" t="s">
         <v>125</v>
       </c>
@@ -8605,7 +8604,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="37"/>
+      <c r="A52" s="43"/>
       <c r="B52" s="6" t="s">
         <v>126</v>
       </c>
@@ -8617,7 +8616,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="37" t="s">
+      <c r="A53" s="43" t="s">
         <v>141</v>
       </c>
       <c r="B53" s="6" t="s">
@@ -8631,7 +8630,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="37"/>
+      <c r="A54" s="43"/>
       <c r="B54" s="6" t="s">
         <v>128</v>
       </c>
@@ -8643,7 +8642,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="37"/>
+      <c r="A55" s="43"/>
       <c r="B55" s="6" t="s">
         <v>129</v>
       </c>
@@ -8655,7 +8654,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="37"/>
+      <c r="A56" s="43"/>
       <c r="B56" s="6" t="s">
         <v>130</v>
       </c>
@@ -8667,7 +8666,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="37"/>
+      <c r="A57" s="43"/>
       <c r="B57" s="6" t="s">
         <v>131</v>
       </c>
@@ -8679,7 +8678,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="37"/>
+      <c r="A58" s="43"/>
       <c r="B58" s="6" t="s">
         <v>132</v>
       </c>
@@ -8691,7 +8690,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="37" t="s">
+      <c r="A59" s="43" t="s">
         <v>142</v>
       </c>
       <c r="B59" s="6" t="s">
@@ -8705,7 +8704,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="37"/>
+      <c r="A60" s="43"/>
       <c r="B60" s="6" t="s">
         <v>134</v>
       </c>
@@ -8728,17 +8727,17 @@
     <mergeCell ref="A50:A52"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:D60">
-    <cfRule type="expression" dxfId="13" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$D$4&lt;&gt;FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:D4">
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$D$4=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$D$4=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8795,7 +8794,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="43" t="s">
         <v>145</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -8809,7 +8808,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
+      <c r="A6" s="43"/>
       <c r="B6" s="6" t="s">
         <v>157</v>
       </c>
@@ -8821,7 +8820,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="6" t="s">
         <v>158</v>
       </c>
@@ -8833,7 +8832,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="6" t="s">
         <v>159</v>
       </c>
@@ -8845,7 +8844,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="6" t="s">
         <v>160</v>
       </c>
@@ -8857,7 +8856,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="6" t="s">
         <v>161</v>
       </c>
@@ -8869,7 +8868,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="43" t="s">
         <v>146</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -8883,7 +8882,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="6" t="s">
         <v>163</v>
       </c>
@@ -8895,7 +8894,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="6" t="s">
         <v>164</v>
       </c>
@@ -8907,7 +8906,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="6" t="s">
         <v>165</v>
       </c>
@@ -8924,17 +8923,17 @@
     <mergeCell ref="A5:A10"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:D4">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$D$4=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$D$4=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:D14">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$D$4&lt;&gt;FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8951,6 +8950,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -9102,15 +9110,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
@@ -9123,6 +9122,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9136,14 +9143,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Testing of fault case creation added
</commit_message>
<xml_diff>
--- a/tests/test_files/Inputs.xlsx
+++ b/tests/test_files/Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD719B77-35DA-4471-98FE-A68C5833616F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C6DB8F-3C92-4425-805A-5779BE6D7773}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -353,7 +353,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="233">
   <si>
     <t>Name</t>
   </si>
@@ -1028,6 +1028,30 @@
   </si>
   <si>
     <t>Switch_210309</t>
+  </si>
+  <si>
+    <t>TEST Cont NC</t>
+  </si>
+  <si>
+    <t>Switch_210264</t>
+  </si>
+  <si>
+    <t>Switch_3045571</t>
+  </si>
+  <si>
+    <t>KERANG 220KV</t>
+  </si>
+  <si>
+    <t>Switch_3931660</t>
+  </si>
+  <si>
+    <t>WEMEN</t>
+  </si>
+  <si>
+    <t>Switch_2479911</t>
+  </si>
+  <si>
+    <t>BALRANALD 220/22KV SUBSTATION</t>
   </si>
 </sst>
 </file>
@@ -2240,7 +2264,7 @@
   <dimension ref="A1:AB166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2492,19 +2516,45 @@
       <c r="AB7" s="3"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>222</v>
+      </c>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
@@ -8950,15 +9000,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -9110,6 +9151,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
@@ -9122,14 +9172,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9143,6 +9185,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Script to create find and create references to terminals for adding to results files
</commit_message>
<xml_diff>
--- a/tests/test_files/Inputs.xlsx
+++ b/tests/test_files/Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C6DB8F-3C92-4425-805A-5779BE6D7773}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D5D72F-06CA-4BD9-BF11-97931A8D93D9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -353,7 +353,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="235">
   <si>
     <t>Name</t>
   </si>
@@ -895,9 +895,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>220 kV A1</t>
-  </si>
-  <si>
     <t>Base_Case</t>
   </si>
   <si>
@@ -922,12 +919,6 @@
     <t>Reference Busbar (NetElements\Substation\Terminal)</t>
   </si>
   <si>
-    <t>Woodland</t>
-  </si>
-  <si>
-    <t>Dunstown</t>
-  </si>
-  <si>
     <t>Automatic Tap Adjustment of Phase Shifters</t>
   </si>
   <si>
@@ -1052,6 +1043,21 @@
   </si>
   <si>
     <t>BALRANALD 220/22KV SUBSTATION</t>
+  </si>
+  <si>
+    <t>CRANBOURNE 220KV</t>
+  </si>
+  <si>
+    <t>2958760_CBTS_7MN2</t>
+  </si>
+  <si>
+    <t>2958762_CBTS_7TB2</t>
+  </si>
+  <si>
+    <t>DEDERANG 330KV</t>
+  </si>
+  <si>
+    <t>1938572_DDTS_5C2</t>
   </si>
 </sst>
 </file>
@@ -1459,7 +1465,21 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -1880,7 +1900,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1890,7 +1910,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1912,7 +1932,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C7" s="4">
         <v>43954</v>
@@ -1972,7 +1992,7 @@
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1987,32 +2007,32 @@
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>178</v>
@@ -2042,13 +2062,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B10" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2129,30 +2149,30 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2263,7 +2283,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AB166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
@@ -2289,13 +2309,13 @@
     </row>
     <row r="3" spans="1:28" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D3" s="1" t="b">
         <v>0</v>
@@ -2303,7 +2323,7 @@
     </row>
     <row r="4" spans="1:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="30" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B4" s="40" t="s">
         <v>9</v>
@@ -2439,7 +2459,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -2473,25 +2493,25 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>224</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
@@ -2517,43 +2537,43 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="L8" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="J8" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="L8" s="19" t="s">
-        <v>231</v>
-      </c>
       <c r="M8" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
@@ -7328,17 +7348,17 @@
     <mergeCell ref="T4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:D3">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>$D$3=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$D$3=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:AB166">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>$D$3&lt;&gt;FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7359,7 +7379,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -7392,18 +7412,18 @@
         <v>20</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>189</v>
+        <v>230</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>189</v>
+        <v>230</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>180</v>
+        <v>231</v>
       </c>
       <c r="D5" s="3" t="b">
         <v>0</v>
@@ -7411,23 +7431,31 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>190</v>
+        <v>230</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>190</v>
+        <v>230</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>180</v>
+        <v>232</v>
       </c>
       <c r="D6" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D7" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -8010,14 +8038,24 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:A8">
     <sortCondition ref="A5:A8"/>
   </sortState>
-  <conditionalFormatting sqref="A5:A103">
-    <cfRule type="expression" dxfId="7" priority="3">
+  <conditionalFormatting sqref="A5:A6 A8:A103">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>LEN(A5)&gt;19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>A3="NAMES OKAY"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>LEN(A7)&gt;19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>LEN(B7)&gt;19</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8059,16 +8097,16 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>196</v>
-      </c>
       <c r="C4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E4" s="1" t="str">
         <f>IF($D$4="","&lt;--- Cannot be empty, please enter False","")</f>
@@ -8118,10 +8156,10 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="43"/>
       <c r="B8" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -8252,13 +8290,13 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="43"/>
       <c r="B19" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>143</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -8777,17 +8815,17 @@
     <mergeCell ref="A50:A52"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:D60">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$D$4&lt;&gt;FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:D4">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$D$4=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$D$4=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8831,16 +8869,16 @@
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C4" t="s">
         <v>210</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="D4" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="C4" t="s">
-        <v>213</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -8851,7 +8889,7 @@
         <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D5" s="8">
         <v>50</v>
@@ -8973,17 +9011,17 @@
     <mergeCell ref="A5:A10"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:D4">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>$D$4=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$D$4=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:D14">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$D$4&lt;&gt;FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9000,6 +9038,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -9151,15 +9198,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
@@ -9172,6 +9210,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9185,14 +9231,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated to process results correctly, just need to finalise a calling script and processing of results.
</commit_message>
<xml_diff>
--- a/tests/test_files/Inputs.xlsx
+++ b/tests/test_files/Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D5D72F-06CA-4BD9-BF11-97931A8D93D9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0CE4EA-9BEE-4F14-AD37-884EF4E9874D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -353,7 +353,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="239">
   <si>
     <t>Name</t>
   </si>
@@ -895,169 +895,181 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Mutual</t>
+  </si>
+  <si>
+    <t>David Mills (PSC)</t>
+  </si>
+  <si>
+    <t>D:\Users\david\Desktop\</t>
+  </si>
+  <si>
+    <t>True = Export the results to Excel (Can be done later)</t>
+  </si>
+  <si>
+    <t>BASE</t>
+  </si>
+  <si>
+    <t>EirGrid\Turlough Hill\220 kV T2001/2 TCB</t>
+  </si>
+  <si>
+    <t>Reference Busbar (NetElements\Substation\Terminal)</t>
+  </si>
+  <si>
+    <t>Automatic Tap Adjustment of Phase Shifters</t>
+  </si>
+  <si>
+    <t>ldf.iPST_at</t>
+  </si>
+  <si>
+    <t>Study Case Load Flow Settings</t>
+  </si>
+  <si>
+    <t>.ComLdf</t>
+  </si>
+  <si>
+    <t>Load Flow Calculation</t>
+  </si>
+  <si>
+    <t>Name of load flow settings to be used for studycase (leave empty to use settings below)</t>
+  </si>
+  <si>
+    <t>PSC Harmonics Input Spreadsheet</t>
+  </si>
+  <si>
+    <t>This is used to carry out multiple frequency scans of a system using PowerFactory</t>
+  </si>
+  <si>
+    <t>Default folder to store log messages and the excel results, this can be overwritten using the GUI and if blank uses the current working directory ie where the script is stored.</t>
+  </si>
+  <si>
+    <t>This sheet can be populated with settings to control some of the inputs and exports from the study that is about to be run. Some of these settings are configurable as part of the GUI</t>
+  </si>
+  <si>
+    <t>Name of exported excel result file (unique time and date of the study is appended to end).</t>
+  </si>
+  <si>
+    <t>Results_Export_Folder</t>
+  </si>
+  <si>
+    <t>Excel_Results</t>
+  </si>
+  <si>
+    <t>Net_Elm</t>
+  </si>
+  <si>
+    <t>Export_to_Excel</t>
+  </si>
+  <si>
+    <t>NSW.ElmNet</t>
+  </si>
+  <si>
+    <t>High Load Case</t>
+  </si>
+  <si>
+    <t>HighLoadTap_testing</t>
+  </si>
+  <si>
+    <t>pscharmonics_test_model</t>
+  </si>
+  <si>
+    <t>Study Case Frequency Sweep</t>
+  </si>
+  <si>
+    <t>Name of frequency scan settings to be used for studycase (leave empty to use settings below)</t>
+  </si>
+  <si>
+    <t>frq.fnom</t>
+  </si>
+  <si>
+    <t>ComFsweep</t>
+  </si>
+  <si>
+    <t>Frequency Sweep</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Contingency Analysis</t>
+  </si>
+  <si>
+    <t>.ComSimoutage</t>
+  </si>
+  <si>
+    <t>Name of existing contingency analysis command that includes details of all of the contingencies to be considered (Set to FALSE if not using)</t>
+  </si>
+  <si>
+    <t>TEST Cont</t>
+  </si>
+  <si>
+    <t>ALBURY 132KV</t>
+  </si>
+  <si>
+    <t>Switch_213211</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>LADBROKE GROVE 132KV</t>
+  </si>
+  <si>
+    <t>Switch_210309</t>
+  </si>
+  <si>
+    <t>TEST Cont NC</t>
+  </si>
+  <si>
+    <t>Switch_210264</t>
+  </si>
+  <si>
+    <t>Switch_3045571</t>
+  </si>
+  <si>
+    <t>KERANG 220KV</t>
+  </si>
+  <si>
+    <t>Switch_3931660</t>
+  </si>
+  <si>
+    <t>WEMEN</t>
+  </si>
+  <si>
+    <t>Switch_2479911</t>
+  </si>
+  <si>
+    <t>BALRANALD 220/22KV SUBSTATION</t>
+  </si>
+  <si>
+    <t>CRANBOURNE 220KV</t>
+  </si>
+  <si>
+    <t>2958760_CBTS_7MN2</t>
+  </si>
+  <si>
+    <t>2958762_CBTS_7TB2</t>
+  </si>
+  <si>
+    <t>DEDERANG 330KV</t>
+  </si>
+  <si>
+    <t>1938572_DDTS_5C2</t>
+  </si>
+  <si>
+    <t>LADBROKE GROVE</t>
+  </si>
+  <si>
+    <t>375520_LADB_G_1T1</t>
+  </si>
+  <si>
     <t>Base_Case</t>
   </si>
   <si>
-    <t>Mutual</t>
-  </si>
-  <si>
-    <t>David Mills (PSC)</t>
-  </si>
-  <si>
-    <t>D:\Users\david\Desktop\</t>
-  </si>
-  <si>
-    <t>True = Export the results to Excel (Can be done later)</t>
-  </si>
-  <si>
-    <t>BASE</t>
-  </si>
-  <si>
-    <t>EirGrid\Turlough Hill\220 kV T2001/2 TCB</t>
-  </si>
-  <si>
-    <t>Reference Busbar (NetElements\Substation\Terminal)</t>
-  </si>
-  <si>
-    <t>Automatic Tap Adjustment of Phase Shifters</t>
-  </si>
-  <si>
-    <t>ldf.iPST_at</t>
-  </si>
-  <si>
-    <t>Study Case Load Flow Settings</t>
-  </si>
-  <si>
-    <t>.ComLdf</t>
-  </si>
-  <si>
-    <t>Load Flow Calculation</t>
-  </si>
-  <si>
-    <t>Name of load flow settings to be used for studycase (leave empty to use settings below)</t>
-  </si>
-  <si>
-    <t>PSC Harmonics Input Spreadsheet</t>
-  </si>
-  <si>
-    <t>This is used to carry out multiple frequency scans of a system using PowerFactory</t>
-  </si>
-  <si>
-    <t>Default folder to store log messages and the excel results, this can be overwritten using the GUI and if blank uses the current working directory ie where the script is stored.</t>
-  </si>
-  <si>
-    <t>This sheet can be populated with settings to control some of the inputs and exports from the study that is about to be run. Some of these settings are configurable as part of the GUI</t>
-  </si>
-  <si>
-    <t>Name of exported excel result file (unique time and date of the study is appended to end).</t>
-  </si>
-  <si>
-    <t>Results_Export_Folder</t>
-  </si>
-  <si>
-    <t>Excel_Results</t>
-  </si>
-  <si>
-    <t>Net_Elm</t>
-  </si>
-  <si>
-    <t>Export_to_Excel</t>
-  </si>
-  <si>
-    <t>NSW.ElmNet</t>
-  </si>
-  <si>
-    <t>High Load Case</t>
-  </si>
-  <si>
-    <t>HighLoadTap_testing</t>
-  </si>
-  <si>
-    <t>pscharmonics_test_model</t>
-  </si>
-  <si>
-    <t>Study Case Frequency Sweep</t>
-  </si>
-  <si>
-    <t>Name of frequency scan settings to be used for studycase (leave empty to use settings below)</t>
-  </si>
-  <si>
-    <t>frq.fnom</t>
-  </si>
-  <si>
-    <t>ComFsweep</t>
-  </si>
-  <si>
-    <t>Frequency Sweep</t>
-  </si>
-  <si>
-    <t>General</t>
-  </si>
-  <si>
-    <t>Contingency Analysis</t>
-  </si>
-  <si>
-    <t>.ComSimoutage</t>
-  </si>
-  <si>
-    <t>Name of existing contingency analysis command that includes details of all of the contingencies to be considered (Set to FALSE if not using)</t>
-  </si>
-  <si>
-    <t>TEST Cont</t>
-  </si>
-  <si>
-    <t>ALBURY 132KV</t>
-  </si>
-  <si>
-    <t>Switch_213211</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
-    <t>LADBROKE GROVE 132KV</t>
-  </si>
-  <si>
-    <t>Switch_210309</t>
-  </si>
-  <si>
-    <t>TEST Cont NC</t>
-  </si>
-  <si>
-    <t>Switch_210264</t>
-  </si>
-  <si>
-    <t>Switch_3045571</t>
-  </si>
-  <si>
-    <t>KERANG 220KV</t>
-  </si>
-  <si>
-    <t>Switch_3931660</t>
-  </si>
-  <si>
-    <t>WEMEN</t>
-  </si>
-  <si>
-    <t>Switch_2479911</t>
-  </si>
-  <si>
-    <t>BALRANALD 220/22KV SUBSTATION</t>
-  </si>
-  <si>
-    <t>CRANBOURNE 220KV</t>
-  </si>
-  <si>
-    <t>2958760_CBTS_7MN2</t>
-  </si>
-  <si>
-    <t>2958762_CBTS_7TB2</t>
-  </si>
-  <si>
-    <t>DEDERANG 330KV</t>
-  </si>
-  <si>
-    <t>1938572_DDTS_5C2</t>
+    <t>Include_Intact</t>
+  </si>
+  <si>
+    <t>True = Will include an additional result for the intact system</t>
   </si>
 </sst>
 </file>
@@ -1467,20 +1479,6 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
       </font>
@@ -1513,6 +1511,20 @@
       <font>
         <color theme="0" tint="-0.499984740745262"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1900,7 +1912,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1910,7 +1922,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1932,7 +1944,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C7" s="4">
         <v>43954</v>
@@ -1971,10 +1983,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1992,7 +2004,7 @@
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2007,32 +2019,32 @@
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>178</v>
@@ -2062,13 +2074,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B10" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2091,6 +2103,17 @@
       </c>
       <c r="C12" s="13" t="s">
         <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="B13" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -2149,30 +2172,30 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C5" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="D5" s="24" t="s">
         <v>204</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C6" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>204</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2284,7 +2307,7 @@
   <dimension ref="A1:AB166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2309,13 +2332,13 @@
     </row>
     <row r="3" spans="1:28" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" t="s">
         <v>213</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="C3" t="s">
-        <v>214</v>
       </c>
       <c r="D3" s="1" t="b">
         <v>0</v>
@@ -2323,7 +2346,7 @@
     </row>
     <row r="4" spans="1:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B4" s="40" t="s">
         <v>9</v>
@@ -2459,7 +2482,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>180</v>
+        <v>236</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -2493,25 +2516,25 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>221</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
@@ -2537,43 +2560,43 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="D8" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="I8" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="H8" s="19" t="s">
+      <c r="J8" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="L8" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="I8" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="J8" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="L8" s="19" t="s">
-        <v>228</v>
-      </c>
       <c r="M8" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
@@ -7379,8 +7402,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7412,18 +7435,18 @@
         <v>20</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D5" s="3" t="b">
         <v>0</v>
@@ -7431,13 +7454,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D6" s="3" t="b">
         <v>0</v>
@@ -7445,23 +7468,31 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>234</v>
       </c>
       <c r="D7" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D8" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -8049,12 +8080,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>LEN(A7)&gt;19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>LEN(B7)&gt;19</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8097,16 +8128,16 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4" t="s">
         <v>190</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="E4" s="1" t="str">
         <f>IF($D$4="","&lt;--- Cannot be empty, please enter False","")</f>
@@ -8156,10 +8187,10 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="43"/>
       <c r="B8" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8" t="s">
         <v>188</v>
-      </c>
-      <c r="C8" t="s">
-        <v>189</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -8290,13 +8321,13 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="43"/>
       <c r="B19" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>143</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -8815,17 +8846,17 @@
     <mergeCell ref="A50:A52"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:D60">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$D$4&lt;&gt;FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:D4">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$D$4=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$D$4=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8869,16 +8900,16 @@
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>208</v>
-      </c>
       <c r="C4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -8889,7 +8920,7 @@
         <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D5" s="8">
         <v>50</v>
@@ -9011,17 +9042,17 @@
     <mergeCell ref="A5:A10"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:D4">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$D$4=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$D$4=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:D14">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$D$4&lt;&gt;FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Creation of batch method for running by AEMO
</commit_message>
<xml_diff>
--- a/tests/test_files/Inputs.xlsx
+++ b/tests/test_files/Inputs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0CE4EA-9BEE-4F14-AD37-884EF4E9874D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F36F7E4-413E-45C5-8030-2DA904CB4A23}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -353,7 +353,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="235">
   <si>
     <t>Name</t>
   </si>
@@ -376,9 +376,6 @@
     <t>Created</t>
   </si>
   <si>
-    <t>v1</t>
-  </si>
-  <si>
     <t>Database</t>
   </si>
   <si>
@@ -859,9 +856,6 @@
     <t>ldf</t>
   </si>
   <si>
-    <t>Recommended Settings</t>
-  </si>
-  <si>
     <t>Pre_Case_Check</t>
   </si>
   <si>
@@ -889,9 +883,6 @@
     <t>Calculation method (0 Balanced AC, 1 Unbalanced AC, 2 DC)</t>
   </si>
   <si>
-    <t>The name of the network elements in PowerFactory. Note this is Case sensitive.</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -955,15 +946,9 @@
     <t>Excel_Results</t>
   </si>
   <si>
-    <t>Net_Elm</t>
-  </si>
-  <si>
     <t>Export_to_Excel</t>
   </si>
   <si>
-    <t>NSW.ElmNet</t>
-  </si>
-  <si>
     <t>High Load Case</t>
   </si>
   <si>
@@ -1070,6 +1055,9 @@
   </si>
   <si>
     <t>True = Will include an additional result for the intact system</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
   </si>
 </sst>
 </file>
@@ -1386,7 +1374,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1471,6 +1459,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1900,7 +1889,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1912,7 +1901,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1922,7 +1911,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1944,13 +1933,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C7" s="4">
-        <v>43954</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
+        <v>43977</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1983,10 +1972,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,12 +1988,12 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2012,108 +2001,92 @@
       <c r="E3" s="36"/>
       <c r="F3" s="36"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>168</v>
-      </c>
-    </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>178</v>
+        <v>167</v>
+      </c>
+      <c r="B7" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="B9" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="B8" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="B9" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>201</v>
       </c>
       <c r="B10" s="14" t="b">
         <v>1</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>171</v>
+      <c r="A11" s="15" t="s">
+        <v>170</v>
       </c>
       <c r="B11" s="14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>172</v>
+        <v>232</v>
       </c>
       <c r="B12" s="14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="B13" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2121,7 +2094,7 @@
     <mergeCell ref="D3:F3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B12" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B11" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2149,7 +2122,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2161,41 +2134,41 @@
         <v>0</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>26</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2324,7 +2297,7 @@
   <sheetData>
     <row r="1" spans="1:28" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="21" x14ac:dyDescent="0.35">
@@ -2332,13 +2305,13 @@
     </row>
     <row r="3" spans="1:28" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D3" s="1" t="b">
         <v>0</v>
@@ -2346,50 +2319,50 @@
     </row>
     <row r="4" spans="1:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="30" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="41"/>
       <c r="D4" s="42"/>
       <c r="E4" s="37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="38"/>
       <c r="G4" s="39"/>
       <c r="H4" s="37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I4" s="38"/>
       <c r="J4" s="39"/>
       <c r="K4" s="37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L4" s="38"/>
       <c r="M4" s="39"/>
       <c r="N4" s="37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O4" s="38"/>
       <c r="P4" s="39"/>
       <c r="Q4" s="37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R4" s="38"/>
       <c r="S4" s="39"/>
       <c r="T4" s="37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U4" s="38"/>
       <c r="V4" s="39"/>
       <c r="W4" s="37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="X4" s="38"/>
       <c r="Y4" s="39"/>
       <c r="Z4" s="37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA4" s="38"/>
       <c r="AB4" s="39"/>
@@ -2399,90 +2372,90 @@
         <v>0</v>
       </c>
       <c r="B5" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="33" t="s">
-        <v>19</v>
-      </c>
       <c r="D5" s="34" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E5" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="34" t="s">
-        <v>19</v>
-      </c>
       <c r="G5" s="34" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H5" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="34" t="s">
-        <v>19</v>
-      </c>
       <c r="J5" s="34" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="K5" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="34" t="s">
-        <v>19</v>
-      </c>
       <c r="M5" s="34" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="N5" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="O5" s="34" t="s">
-        <v>19</v>
-      </c>
       <c r="P5" s="34" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="Q5" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="R5" s="34" t="s">
-        <v>19</v>
-      </c>
       <c r="S5" s="34" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="T5" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="U5" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="U5" s="34" t="s">
-        <v>19</v>
-      </c>
       <c r="V5" s="34" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="W5" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="X5" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="X5" s="34" t="s">
-        <v>19</v>
-      </c>
       <c r="Y5" s="34" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="Z5" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA5" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="AA5" s="34" t="s">
-        <v>19</v>
-      </c>
       <c r="AB5" s="34" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -2516,25 +2489,25 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
@@ -2560,43 +2533,43 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="H8" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="I8" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="L8" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>225</v>
-      </c>
-      <c r="J8" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="L8" s="19" t="s">
-        <v>227</v>
-      </c>
       <c r="M8" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
@@ -7415,7 +7388,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7429,24 +7402,24 @@
         <v>0</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D5" s="3" t="b">
         <v>0</v>
@@ -7454,13 +7427,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D6" s="3" t="b">
         <v>0</v>
@@ -7468,13 +7441,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D7" s="3" t="b">
         <v>1</v>
@@ -7482,13 +7455,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D8" s="3" t="b">
         <v>0</v>
@@ -8122,22 +8095,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="7"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>192</v>
-      </c>
       <c r="C4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E4" s="1" t="str">
         <f>IF($D$4="","&lt;--- Cannot be empty, please enter False","")</f>
@@ -8148,13 +8121,13 @@
     </row>
     <row r="5" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -8163,10 +8136,10 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="43"/>
       <c r="B6" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -8175,10 +8148,10 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="43"/>
       <c r="B7" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -8187,10 +8160,10 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="43"/>
       <c r="B8" s="6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -8199,10 +8172,10 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="43"/>
       <c r="B9" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -8211,10 +8184,10 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="43"/>
       <c r="B10" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -8223,10 +8196,10 @@
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="43"/>
       <c r="B11" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -8235,10 +8208,10 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="43"/>
       <c r="B12" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -8247,10 +8220,10 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="43"/>
       <c r="B13" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -8259,10 +8232,10 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="43"/>
       <c r="B14" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -8271,10 +8244,10 @@
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="43"/>
       <c r="B15" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15">
         <v>100</v>
@@ -8282,13 +8255,13 @@
     </row>
     <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -8297,10 +8270,10 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="43"/>
       <c r="B17" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -8309,10 +8282,10 @@
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="43"/>
       <c r="B18" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -8321,22 +8294,22 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="43"/>
       <c r="B19" s="9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="43"/>
       <c r="B20" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -8344,13 +8317,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -8359,10 +8332,10 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="43"/>
       <c r="B22" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -8371,10 +8344,10 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="43"/>
       <c r="B23" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -8383,10 +8356,10 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="43"/>
       <c r="B24" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -8395,10 +8368,10 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="43"/>
       <c r="B25" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25">
         <v>20</v>
@@ -8407,10 +8380,10 @@
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="43"/>
       <c r="B26" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -8419,10 +8392,10 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="43"/>
       <c r="B27" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -8431,10 +8404,10 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="43"/>
       <c r="B28" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -8443,10 +8416,10 @@
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="43"/>
       <c r="B29" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D29">
         <v>2</v>
@@ -8455,10 +8428,10 @@
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="43"/>
       <c r="B30" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -8467,10 +8440,10 @@
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="43"/>
       <c r="B31" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -8478,13 +8451,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D32">
         <v>100</v>
@@ -8493,10 +8466,10 @@
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="43"/>
       <c r="B33" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33">
         <v>80</v>
@@ -8505,10 +8478,10 @@
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="43"/>
       <c r="B34" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34">
         <v>5</v>
@@ -8517,10 +8490,10 @@
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="43"/>
       <c r="B35" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D35">
         <v>10000</v>
@@ -8529,10 +8502,10 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="43"/>
       <c r="B36" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D36">
         <v>10</v>
@@ -8541,10 +8514,10 @@
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="43"/>
       <c r="B37" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -8553,10 +8526,10 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="43"/>
       <c r="B38" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -8565,10 +8538,10 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="43"/>
       <c r="B39" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -8576,13 +8549,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="43" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -8591,10 +8564,10 @@
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="43"/>
       <c r="B41" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -8603,10 +8576,10 @@
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="43"/>
       <c r="B42" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D42">
         <v>2</v>
@@ -8615,10 +8588,10 @@
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="43"/>
       <c r="B43" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -8627,10 +8600,10 @@
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="43"/>
       <c r="B44" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D44">
         <v>110</v>
@@ -8639,10 +8612,10 @@
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="43"/>
       <c r="B45" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D45">
         <v>0.9</v>
@@ -8651,10 +8624,10 @@
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="43"/>
       <c r="B46" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D46">
         <v>1.1200000000000001</v>
@@ -8663,22 +8636,22 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="43"/>
       <c r="B47" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="43"/>
       <c r="B48" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -8687,24 +8660,24 @@
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="43"/>
       <c r="B49" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="43" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D50">
         <v>100</v>
@@ -8713,10 +8686,10 @@
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="43"/>
       <c r="B51" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D51">
         <v>100</v>
@@ -8725,10 +8698,10 @@
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="43"/>
       <c r="B52" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D52">
         <v>100</v>
@@ -8736,13 +8709,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="43" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -8751,10 +8724,10 @@
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="43"/>
       <c r="B54" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D54">
         <v>0.9</v>
@@ -8763,10 +8736,10 @@
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="43"/>
       <c r="B55" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D55">
         <v>12</v>
@@ -8775,10 +8748,10 @@
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="43"/>
       <c r="B56" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D56">
         <v>0.95</v>
@@ -8787,10 +8760,10 @@
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="43"/>
       <c r="B57" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D57">
         <v>0.1</v>
@@ -8799,10 +8772,10 @@
     <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="43"/>
       <c r="B58" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -8810,13 +8783,13 @@
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="43" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -8825,10 +8798,10 @@
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="43"/>
       <c r="B60" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -8894,33 +8867,33 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="7"/>
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C4" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D5" s="8">
         <v>50</v>
@@ -8929,10 +8902,10 @@
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="43"/>
       <c r="B6" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -8941,10 +8914,10 @@
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="43"/>
       <c r="B7" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D7" s="8">
         <v>50</v>
@@ -8953,10 +8926,10 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="43"/>
       <c r="B8" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D8" s="8">
         <v>500</v>
@@ -8965,10 +8938,10 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="43"/>
       <c r="B9" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D9">
         <v>50</v>
@@ -8977,10 +8950,10 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="43"/>
       <c r="B10" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -8988,13 +8961,13 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="43" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D11">
         <v>0.01</v>
@@ -9003,10 +8976,10 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="43"/>
       <c r="B12" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D12">
         <v>5.0000000000000001E-3</v>
@@ -9015,10 +8988,10 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="43"/>
       <c r="B13" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -9027,10 +9000,10 @@
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="43"/>
       <c r="B14" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -9069,15 +9042,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -9229,6 +9193,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
@@ -9241,14 +9214,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9262,6 +9227,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updates to test files for input testing prior to processing of outputs
</commit_message>
<xml_diff>
--- a/tests/test_files/Inputs.xlsx
+++ b/tests/test_files/Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F36F7E4-413E-45C5-8030-2DA904CB4A23}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2A922F-BB3E-41F0-A9BE-0D7787F49D27}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28365" yWindow="1350" windowWidth="21600" windowHeight="11385" tabRatio="868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -1435,6 +1435,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1459,7 +1460,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1938,7 +1938,7 @@
       <c r="C7" s="4">
         <v>43977</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="36" t="s">
         <v>234</v>
       </c>
     </row>
@@ -1974,7 +1974,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1997,9 +1997,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
@@ -2279,8 +2279,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AB166"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,51 +2321,51 @@
       <c r="A4" s="30" t="s">
         <v>206</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="37" t="s">
+      <c r="C4" s="42"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="37" t="s">
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="38"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="37" t="s">
+      <c r="I4" s="39"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="38"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="37" t="s">
+      <c r="L4" s="39"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="38"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="37" t="s">
+      <c r="O4" s="39"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="R4" s="38"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="37" t="s">
+      <c r="R4" s="39"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="U4" s="38"/>
-      <c r="V4" s="39"/>
-      <c r="W4" s="37" t="s">
+      <c r="U4" s="39"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="38"/>
-      <c r="Y4" s="39"/>
-      <c r="Z4" s="37" t="s">
+      <c r="X4" s="39"/>
+      <c r="Y4" s="40"/>
+      <c r="Z4" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="AA4" s="38"/>
-      <c r="AB4" s="39"/>
+      <c r="AA4" s="39"/>
+      <c r="AB4" s="40"/>
     </row>
     <row r="5" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
@@ -8120,7 +8120,7 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="44" t="s">
         <v>134</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -8134,7 +8134,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="6" t="s">
         <v>81</v>
       </c>
@@ -8146,7 +8146,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="6" t="s">
         <v>89</v>
       </c>
@@ -8158,7 +8158,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="6" t="s">
         <v>184</v>
       </c>
@@ -8170,7 +8170,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="6" t="s">
         <v>82</v>
       </c>
@@ -8182,7 +8182,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="6" t="s">
         <v>83</v>
       </c>
@@ -8194,7 +8194,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="6" t="s">
         <v>90</v>
       </c>
@@ -8206,7 +8206,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="6" t="s">
         <v>84</v>
       </c>
@@ -8218,7 +8218,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="6" t="s">
         <v>85</v>
       </c>
@@ -8230,7 +8230,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="6" t="s">
         <v>86</v>
       </c>
@@ -8242,7 +8242,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="6" t="s">
         <v>87</v>
       </c>
@@ -8254,7 +8254,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="44" t="s">
         <v>135</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -8268,7 +8268,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="6" t="s">
         <v>91</v>
       </c>
@@ -8280,7 +8280,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="6" t="s">
         <v>92</v>
       </c>
@@ -8292,7 +8292,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="9" t="s">
         <v>183</v>
       </c>
@@ -8304,7 +8304,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="6" t="s">
         <v>93</v>
       </c>
@@ -8316,7 +8316,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="44" t="s">
         <v>136</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -8330,7 +8330,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="6" t="s">
         <v>95</v>
       </c>
@@ -8342,7 +8342,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="6" t="s">
         <v>96</v>
       </c>
@@ -8354,7 +8354,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="6" t="s">
         <v>97</v>
       </c>
@@ -8366,7 +8366,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="6" t="s">
         <v>98</v>
       </c>
@@ -8378,7 +8378,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="43"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="6" t="s">
         <v>99</v>
       </c>
@@ -8390,7 +8390,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="43"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="6" t="s">
         <v>100</v>
       </c>
@@ -8402,7 +8402,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="43"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="6" t="s">
         <v>101</v>
       </c>
@@ -8414,7 +8414,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="43"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="6" t="s">
         <v>102</v>
       </c>
@@ -8426,7 +8426,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="43"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="6" t="s">
         <v>103</v>
       </c>
@@ -8438,7 +8438,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="43"/>
+      <c r="A31" s="44"/>
       <c r="B31" s="6" t="s">
         <v>104</v>
       </c>
@@ -8450,7 +8450,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="44" t="s">
         <v>137</v>
       </c>
       <c r="B32" s="6" t="s">
@@ -8464,7 +8464,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="43"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="6" t="s">
         <v>106</v>
       </c>
@@ -8476,7 +8476,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="43"/>
+      <c r="A34" s="44"/>
       <c r="B34" s="6" t="s">
         <v>107</v>
       </c>
@@ -8488,7 +8488,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="43"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="6" t="s">
         <v>108</v>
       </c>
@@ -8500,7 +8500,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="43"/>
+      <c r="A36" s="44"/>
       <c r="B36" s="6" t="s">
         <v>109</v>
       </c>
@@ -8512,7 +8512,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="43"/>
+      <c r="A37" s="44"/>
       <c r="B37" s="6" t="s">
         <v>110</v>
       </c>
@@ -8524,7 +8524,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="43"/>
+      <c r="A38" s="44"/>
       <c r="B38" s="6" t="s">
         <v>111</v>
       </c>
@@ -8536,7 +8536,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="43"/>
+      <c r="A39" s="44"/>
       <c r="B39" s="6" t="s">
         <v>112</v>
       </c>
@@ -8548,7 +8548,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="43" t="s">
+      <c r="A40" s="44" t="s">
         <v>138</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -8562,7 +8562,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="43"/>
+      <c r="A41" s="44"/>
       <c r="B41" s="6" t="s">
         <v>114</v>
       </c>
@@ -8574,7 +8574,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="43"/>
+      <c r="A42" s="44"/>
       <c r="B42" s="6" t="s">
         <v>115</v>
       </c>
@@ -8586,7 +8586,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="43"/>
+      <c r="A43" s="44"/>
       <c r="B43" s="6" t="s">
         <v>116</v>
       </c>
@@ -8598,7 +8598,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="43"/>
+      <c r="A44" s="44"/>
       <c r="B44" s="6" t="s">
         <v>117</v>
       </c>
@@ -8610,7 +8610,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="43"/>
+      <c r="A45" s="44"/>
       <c r="B45" s="6" t="s">
         <v>118</v>
       </c>
@@ -8622,7 +8622,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="43"/>
+      <c r="A46" s="44"/>
       <c r="B46" s="6" t="s">
         <v>119</v>
       </c>
@@ -8634,7 +8634,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="43"/>
+      <c r="A47" s="44"/>
       <c r="B47" s="9" t="s">
         <v>120</v>
       </c>
@@ -8646,7 +8646,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="43"/>
+      <c r="A48" s="44"/>
       <c r="B48" s="6" t="s">
         <v>121</v>
       </c>
@@ -8658,7 +8658,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="43"/>
+      <c r="A49" s="44"/>
       <c r="B49" s="9" t="s">
         <v>122</v>
       </c>
@@ -8670,7 +8670,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="43" t="s">
+      <c r="A50" s="44" t="s">
         <v>139</v>
       </c>
       <c r="B50" s="6" t="s">
@@ -8684,7 +8684,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="43"/>
+      <c r="A51" s="44"/>
       <c r="B51" s="6" t="s">
         <v>124</v>
       </c>
@@ -8696,7 +8696,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="43"/>
+      <c r="A52" s="44"/>
       <c r="B52" s="6" t="s">
         <v>125</v>
       </c>
@@ -8708,7 +8708,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="43" t="s">
+      <c r="A53" s="44" t="s">
         <v>140</v>
       </c>
       <c r="B53" s="6" t="s">
@@ -8722,7 +8722,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="43"/>
+      <c r="A54" s="44"/>
       <c r="B54" s="6" t="s">
         <v>127</v>
       </c>
@@ -8734,7 +8734,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="43"/>
+      <c r="A55" s="44"/>
       <c r="B55" s="6" t="s">
         <v>128</v>
       </c>
@@ -8746,7 +8746,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="43"/>
+      <c r="A56" s="44"/>
       <c r="B56" s="6" t="s">
         <v>129</v>
       </c>
@@ -8758,7 +8758,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="43"/>
+      <c r="A57" s="44"/>
       <c r="B57" s="6" t="s">
         <v>130</v>
       </c>
@@ -8770,7 +8770,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="43"/>
+      <c r="A58" s="44"/>
       <c r="B58" s="6" t="s">
         <v>131</v>
       </c>
@@ -8782,7 +8782,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="43" t="s">
+      <c r="A59" s="44" t="s">
         <v>141</v>
       </c>
       <c r="B59" s="6" t="s">
@@ -8796,7 +8796,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="43"/>
+      <c r="A60" s="44"/>
       <c r="B60" s="6" t="s">
         <v>133</v>
       </c>
@@ -8886,7 +8886,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="44" t="s">
         <v>144</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -8900,7 +8900,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="6" t="s">
         <v>156</v>
       </c>
@@ -8912,7 +8912,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="6" t="s">
         <v>157</v>
       </c>
@@ -8924,7 +8924,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="6" t="s">
         <v>158</v>
       </c>
@@ -8936,7 +8936,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="6" t="s">
         <v>159</v>
       </c>
@@ -8948,7 +8948,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="6" t="s">
         <v>160</v>
       </c>
@@ -8960,7 +8960,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="44" t="s">
         <v>145</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -8974,7 +8974,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="6" t="s">
         <v>162</v>
       </c>
@@ -8986,7 +8986,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="6" t="s">
         <v>163</v>
       </c>
@@ -8998,7 +8998,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="6" t="s">
         <v>164</v>
       </c>
@@ -9042,6 +9042,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -9193,15 +9202,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
@@ -9214,6 +9214,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9227,14 +9235,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updates to resolve running in Batch Mode queries by AEMO
</commit_message>
<xml_diff>
--- a/tests/test_files/Inputs.xlsx
+++ b/tests/test_files/Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD2B5E8-11BB-4899-BCA1-AA5B08159ADB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F2FFE3-83FF-47A9-BAAE-82EB4A8FEA96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="814" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -175,6 +175,438 @@
         </r>
       </text>
     </comment>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{A71363A8-65B2-45DF-B222-5FEB8C1F497A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element for substation with ending '.ElmSwitch'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{3E6D1FBA-8D4C-472E-B978-795746F1E8B1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element in substation that has ending '.ElmCoup'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{AC2F622F-0EAE-4D9F-8268-19F08F608DB2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element for substation with ending '.ElmSwitch'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{C8EBD9C2-2265-4414-8437-073EE4C373E1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element in substation that has ending '.ElmCoup'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{D756CFE5-F56A-4945-B442-CA4E7FB24505}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element for substation with ending '.ElmSwitch'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{276C2315-543F-4A20-A1F2-00D0BFA3D969}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element in substation that has ending '.ElmCoup'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K5" authorId="0" shapeId="0" xr:uid="{2DDD6917-9195-462B-905E-7D84DC9E0EE4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element for substation with ending '.ElmSwitch'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L5" authorId="0" shapeId="0" xr:uid="{2D0E59A4-CA0B-46DA-83B0-F93D89166674}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element in substation that has ending '.ElmCoup'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N5" authorId="0" shapeId="0" xr:uid="{454D0762-E801-49A8-9036-6FB7A0E3B28D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element for substation with ending '.ElmSwitch'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O5" authorId="0" shapeId="0" xr:uid="{E169F9E7-E998-4449-841B-AFB7FA93660A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element in substation that has ending '.ElmCoup'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{D39B2153-F066-43F5-951A-72502784B79F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element for substation with ending '.ElmSwitch'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{25F55907-781B-40E8-A45E-5102AF235E8D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element in substation that has ending '.ElmCoup'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T5" authorId="0" shapeId="0" xr:uid="{E8A00494-10BD-48DC-B6B8-FB4D8D767B5D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element for substation with ending '.ElmSwitch'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U5" authorId="0" shapeId="0" xr:uid="{DD7BE88D-D67E-40A6-AC6D-92F7F4E8E0B3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element in substation that has ending '.ElmCoup'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W5" authorId="0" shapeId="0" xr:uid="{7367427C-7D63-4E9F-BD78-CDD7995E292A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element for substation with ending '.ElmSwitch'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X5" authorId="0" shapeId="0" xr:uid="{21E38F55-1338-4CA1-BE78-A425E8BCEF95}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element in substation that has ending '.ElmCoup'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z5" authorId="0" shapeId="0" xr:uid="{CB27BF79-49EC-4F01-ACE6-A66511B23660}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element for substation with ending '.ElmSwitch'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA5" authorId="0" shapeId="0" xr:uid="{D154C1E4-8448-4B2E-A33C-AA27B2CF46E7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of PowerFactory element in substation that has ending '.ElmCoup'</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -206,6 +638,222 @@
           </rPr>
           <t xml:space="preserve">
 Either enter the name of a Contingency analysis in the study case (*.ComSimoutage) to use or set to False and use the contingencies described below</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{E8A1C630-46BE-4255-AA45-B44DC55D197E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Element in PowerFactory of either type line (.ElmLne) or type branch (ElmBranch)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{C9EF2244-0586-4B6C-87C4-6624B0B75E61}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Element in PowerFactory of either type line (.ElmLne) or type branch (ElmBranch)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{42A5C3E7-B2EE-4A09-8B7B-E02D317AB9DD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Element in PowerFactory of either type line (.ElmLne) or type branch (ElmBranch)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{ED7EECE0-96CB-44B0-B89D-A343849F0B1C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Element in PowerFactory of either type line (.ElmLne) or type branch (ElmBranch)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{1B7FDBAA-6198-4BCA-8426-9663E7E24894}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Element in PowerFactory of either type line (.ElmLne) or type branch (ElmBranch)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L5" authorId="0" shapeId="0" xr:uid="{FB27C2ED-0C32-4035-833D-1347ABAD801D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Element in PowerFactory of either type line (.ElmLne) or type branch (ElmBranch)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N5" authorId="0" shapeId="0" xr:uid="{2DF45063-E48B-4E78-9E8D-13D188F89E15}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Element in PowerFactory of either type line (.ElmLne) or type branch (ElmBranch)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{44F398E0-28F8-4FE9-BBFC-F7B624D301BE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Element in PowerFactory of either type line (.ElmLne) or type branch (ElmBranch)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{0C526B02-1196-48B5-A497-8CD616A9800A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Element in PowerFactory of either type line (.ElmLne) or type branch (ElmBranch)</t>
         </r>
       </text>
     </comment>
@@ -1122,9 +1770,6 @@
     <t>Line 5</t>
   </si>
   <si>
-    <t>Line Name</t>
-  </si>
-  <si>
     <t>Line 6</t>
   </si>
   <si>
@@ -1165,6 +1810,9 @@
   </si>
   <si>
     <t>3931655_KGTS_WETS_220</t>
+  </si>
+  <si>
+    <t>Line / Branch Name</t>
   </si>
 </sst>
 </file>
@@ -1291,7 +1939,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1465,17 +2113,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -1634,24 +2271,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="2" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="2" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1689,7 +2326,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -1767,7 +2403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
@@ -1785,8 +2421,15 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1808,13 +2451,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1831,26 +2467,6 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="24">
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1922,6 +2538,26 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -2754,7 +3390,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2770,41 +3406,41 @@
       <c r="A1" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="55" t="s">
         <v>221</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="56" t="s">
         <v>219</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="57" t="s">
         <v>178</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="59"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -2850,7 +3486,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>168</v>
@@ -2859,7 +3495,7 @@
         <v>44030</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3036,7 +3672,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3052,125 +3688,125 @@
       <c r="A1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="61" t="s">
         <v>179</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="62"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="62"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
+      <c r="A4" s="61"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="37" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="37" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="B7" s="35" t="b">
+      <c r="B7" s="34" t="b">
         <v>1</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="38" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="B8" s="35" t="b">
+      <c r="B8" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="38" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="B9" s="35" t="b">
+      <c r="B9" s="34" t="b">
         <v>1</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="38" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="B10" s="35" t="b">
+      <c r="B10" s="34" t="b">
         <v>1</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="38" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="B11" s="35" t="b">
+      <c r="B11" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="38" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="35" t="s">
         <v>216</v>
       </c>
-      <c r="B12" s="35" t="b">
+      <c r="B12" s="34" t="b">
         <v>1</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="38" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="B13" s="35" t="b">
+      <c r="B13" s="34" t="b">
         <v>1</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="38" t="s">
         <v>229</v>
       </c>
     </row>
@@ -3224,21 +3860,21 @@
       <c r="A1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="63"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
+      <c r="A2" s="62"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="64"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
     </row>
     <row r="4" spans="1:4" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
@@ -3395,8 +4031,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AB166"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:M9"/>
+    <sheetView topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3416,78 +4052,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
-        <v>241</v>
-      </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
-      <c r="T1" s="61"/>
-      <c r="U1" s="61"/>
-      <c r="V1" s="61"/>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
-      <c r="AA1" s="61"/>
-      <c r="AB1" s="61"/>
+      <c r="A1" s="64" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" s="64"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="60"/>
+      <c r="AB1" s="60"/>
     </row>
     <row r="2" spans="1:28" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="72"/>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="72"/>
-      <c r="R2" s="72"/>
-      <c r="S2" s="72"/>
-      <c r="T2" s="72"/>
-      <c r="U2" s="72"/>
-      <c r="V2" s="72"/>
-      <c r="W2" s="72"/>
-      <c r="X2" s="72"/>
-      <c r="Y2" s="72"/>
-      <c r="Z2" s="72"/>
-      <c r="AA2" s="72"/>
-      <c r="AB2" s="72"/>
+      <c r="A2" s="65"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="65"/>
+      <c r="X2" s="65"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
     </row>
     <row r="3" spans="1:28" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="53" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="54" t="s">
         <v>194</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="54" t="s">
         <v>193</v>
       </c>
-      <c r="D3" s="54" t="b">
+      <c r="D3" s="53" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3495,51 +4131,51 @@
       <c r="A4" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="65" t="s">
+      <c r="C4" s="70"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="65" t="s">
+      <c r="F4" s="67"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="66"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="65" t="s">
+      <c r="I4" s="67"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="66"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="65" t="s">
+      <c r="L4" s="67"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="66"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="65" t="s">
+      <c r="O4" s="67"/>
+      <c r="P4" s="68"/>
+      <c r="Q4" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="R4" s="66"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="65" t="s">
+      <c r="R4" s="67"/>
+      <c r="S4" s="68"/>
+      <c r="T4" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="U4" s="66"/>
-      <c r="V4" s="67"/>
-      <c r="W4" s="65" t="s">
+      <c r="U4" s="67"/>
+      <c r="V4" s="68"/>
+      <c r="W4" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="X4" s="66"/>
-      <c r="Y4" s="67"/>
-      <c r="Z4" s="65" t="s">
+      <c r="X4" s="67"/>
+      <c r="Y4" s="68"/>
+      <c r="Z4" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="AA4" s="66"/>
-      <c r="AB4" s="67"/>
+      <c r="AA4" s="67"/>
+      <c r="AB4" s="68"/>
     </row>
     <row r="5" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
@@ -3554,73 +4190,73 @@
       <c r="D5" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="30" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="30" t="s">
         <v>16</v>
       </c>
       <c r="J5" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="K5" s="32" t="s">
+      <c r="K5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="31" t="s">
+      <c r="L5" s="30" t="s">
         <v>16</v>
       </c>
       <c r="M5" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="N5" s="32" t="s">
+      <c r="N5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="31" t="s">
+      <c r="O5" s="30" t="s">
         <v>16</v>
       </c>
       <c r="P5" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="Q5" s="32" t="s">
+      <c r="Q5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="R5" s="31" t="s">
+      <c r="R5" s="30" t="s">
         <v>16</v>
       </c>
       <c r="S5" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="T5" s="32" t="s">
+      <c r="T5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="U5" s="31" t="s">
+      <c r="U5" s="30" t="s">
         <v>16</v>
       </c>
       <c r="V5" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="W5" s="32" t="s">
+      <c r="W5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="X5" s="31" t="s">
+      <c r="X5" s="30" t="s">
         <v>16</v>
       </c>
       <c r="Y5" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="Z5" s="32" t="s">
+      <c r="Z5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="AA5" s="31" t="s">
+      <c r="AA5" s="30" t="s">
         <v>16</v>
       </c>
       <c r="AB5" s="31" t="s">
@@ -8548,8 +9184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3D923C-DF32-42AB-9854-C26FD0393729}">
   <dimension ref="A1:AB166"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -8571,158 +9207,158 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="84" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="73" t="s">
-        <v>240</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
+      <c r="A1" s="72" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
     </row>
     <row r="2" spans="1:19" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="72"/>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="72"/>
-      <c r="R2" s="72"/>
-      <c r="S2" s="72"/>
+      <c r="A2" s="65"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
     </row>
     <row r="3" spans="1:19" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="53" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="51" t="s">
         <v>194</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="D3" s="51" t="b">
+      <c r="D3" s="50" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="47" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" s="46" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="69" t="s">
         <v>230</v>
       </c>
-      <c r="C4" s="70"/>
-      <c r="D4" s="65" t="s">
+      <c r="C4" s="71"/>
+      <c r="D4" s="66" t="s">
         <v>231</v>
       </c>
-      <c r="E4" s="67"/>
-      <c r="F4" s="65" t="s">
+      <c r="E4" s="68"/>
+      <c r="F4" s="66" t="s">
         <v>232</v>
       </c>
-      <c r="G4" s="67"/>
-      <c r="H4" s="65" t="s">
+      <c r="G4" s="68"/>
+      <c r="H4" s="66" t="s">
         <v>233</v>
       </c>
-      <c r="I4" s="67"/>
-      <c r="J4" s="65" t="s">
+      <c r="I4" s="68"/>
+      <c r="J4" s="66" t="s">
         <v>234</v>
       </c>
-      <c r="K4" s="67"/>
-      <c r="L4" s="65" t="s">
+      <c r="K4" s="68"/>
+      <c r="L4" s="66" t="s">
+        <v>235</v>
+      </c>
+      <c r="M4" s="68"/>
+      <c r="N4" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="M4" s="67"/>
-      <c r="N4" s="65" t="s">
+      <c r="O4" s="68"/>
+      <c r="P4" s="66" t="s">
         <v>237</v>
       </c>
-      <c r="O4" s="67"/>
-      <c r="P4" s="65" t="s">
+      <c r="Q4" s="68"/>
+      <c r="R4" s="66" t="s">
         <v>238</v>
       </c>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="65" t="s">
-        <v>239</v>
-      </c>
-      <c r="S4" s="67"/>
-    </row>
-    <row r="5" spans="1:19" s="47" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="S4" s="68"/>
+    </row>
+    <row r="5" spans="1:19" s="46" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>166</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="E5" s="31" t="s">
         <v>166</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>166</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="I5" s="31" t="s">
         <v>166</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="K5" s="31" t="s">
         <v>166</v>
       </c>
       <c r="L5" s="29" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="M5" s="31" t="s">
         <v>166</v>
       </c>
       <c r="N5" s="29" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="O5" s="31" t="s">
         <v>166</v>
       </c>
       <c r="P5" s="29" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="Q5" s="31" t="s">
         <v>166</v>
       </c>
       <c r="R5" s="29" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="S5" s="31" t="s">
         <v>166</v>
@@ -8733,10 +9369,10 @@
         <v>195</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
@@ -8760,16 +9396,16 @@
         <v>201</v>
       </c>
       <c r="B7" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>242</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>249</v>
-      </c>
       <c r="E7" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
@@ -12151,7 +12787,7 @@
       <formula>$D$3=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:S5 A8:S166 A6:A7 C6:S6 C7 F7:S7">
+  <conditionalFormatting sqref="A8:S166 A6:A7 C6:S6 C7 F7:S7 A4:S5">
     <cfRule type="expression" dxfId="16" priority="16">
       <formula>$D$3&lt;&gt;FALSE</formula>
     </cfRule>
@@ -12162,22 +12798,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="14" priority="4">
       <formula>$D$3&lt;&gt;FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>$D$3&lt;&gt;FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>$D$3&lt;&gt;FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>$D$3&lt;&gt;FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12217,33 +12853,33 @@
       <c r="A1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="60"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="str">
+      <c r="A3" s="41" t="str">
         <f t="array" ref="A3">IF(LEN(A5:A103)&gt;19,"NAME LONG", "NAMES OKAY")</f>
         <v>NAMES OKAY</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="40" t="s">
         <v>167</v>
       </c>
     </row>
@@ -12883,22 +13519,22 @@
     <mergeCell ref="A2:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:A6 A8:A103">
-    <cfRule type="expression" dxfId="14" priority="5">
+    <cfRule type="expression" dxfId="10" priority="5">
       <formula>LEN(A5)&gt;19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="13" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>A3="NAMES OKAY"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>LEN(A7)&gt;19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>LEN(B7)&gt;19</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12914,14 +13550,14 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.5703125" style="15" customWidth="1"/>
-    <col min="2" max="2" width="121.7109375" style="43" customWidth="1"/>
+    <col min="2" max="2" width="121.7109375" style="42" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" style="15" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" style="15" customWidth="1"/>
     <col min="5" max="5" width="13.140625" style="15" hidden="1" customWidth="1"/>
@@ -12938,36 +13574,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="60"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="75" t="str">
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="74" t="str">
         <f>IF($D$4="","Cannot be empty, please enter FALSE","")</f>
         <v/>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="60"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="75"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="74"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="B4" s="43" t="s">
-        <v>246</v>
-      </c>
-      <c r="C4" s="47" t="s">
+      <c r="B4" s="42" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="46" t="s">
         <v>175</v>
       </c>
       <c r="D4" s="17" t="s">
@@ -12977,665 +13613,665 @@
       <c r="G4" s="17"/>
     </row>
     <row r="5" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="73" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="45">
+      <c r="D5" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="74"/>
-      <c r="B6" s="43" t="s">
+      <c r="A6" s="73"/>
+      <c r="B6" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="44">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="74"/>
-      <c r="B7" s="43" t="s">
+      <c r="A7" s="73"/>
+      <c r="B7" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="45">
+      <c r="D7" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="73"/>
+      <c r="B8" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="D8" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="73"/>
+      <c r="B9" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="44">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="74"/>
-      <c r="B8" s="43" t="s">
-        <v>172</v>
-      </c>
-      <c r="C8" s="47" t="s">
-        <v>173</v>
-      </c>
-      <c r="D8" s="45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="73"/>
+      <c r="B10" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="73"/>
+      <c r="B11" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="73"/>
+      <c r="B12" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="73"/>
+      <c r="B13" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="73"/>
+      <c r="B14" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="73"/>
+      <c r="B15" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="73" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="73"/>
+      <c r="B17" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="44">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="74"/>
-      <c r="B9" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="73"/>
+      <c r="B18" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="44">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="74"/>
-      <c r="B10" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="73"/>
+      <c r="B19" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="45"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="73"/>
+      <c r="B20" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="44">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="74"/>
-      <c r="B11" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="73" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="73"/>
+      <c r="B22" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="73"/>
+      <c r="B23" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="44">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="74"/>
-      <c r="B12" s="43" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="73"/>
+      <c r="B24" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="73"/>
+      <c r="B25" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="44">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="73"/>
+      <c r="B26" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="73"/>
+      <c r="B27" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="73"/>
+      <c r="B28" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="73"/>
+      <c r="B29" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="73"/>
+      <c r="B30" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="73"/>
+      <c r="B31" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="73" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="44">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="73"/>
+      <c r="B33" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="44">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="73"/>
+      <c r="B34" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="73"/>
+      <c r="B35" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="73"/>
+      <c r="B36" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="44">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="73"/>
+      <c r="B37" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="73"/>
+      <c r="B38" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="73"/>
+      <c r="B39" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="B40" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="73"/>
+      <c r="B41" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="C41" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="73"/>
+      <c r="B42" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="73"/>
+      <c r="B43" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="73"/>
+      <c r="B44" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" s="44">
         <v>80</v>
       </c>
-      <c r="C12" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="45">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="73"/>
+      <c r="B45" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="C45" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="44">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="73"/>
+      <c r="B46" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" s="44">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="73"/>
+      <c r="B47" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="C47" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47" s="44">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="74"/>
-      <c r="B13" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="B48" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="C48" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" s="44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="73"/>
+      <c r="B49" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" s="44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="73"/>
+      <c r="B50" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" s="44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="C51" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="73"/>
+      <c r="B52" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" s="44">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="73"/>
+      <c r="B53" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="C53" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" s="44">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="73"/>
+      <c r="B54" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" s="44">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="73"/>
+      <c r="B55" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C55" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="D55" s="44">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="73"/>
+      <c r="B56" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="C56" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="73" t="s">
+        <v>135</v>
+      </c>
+      <c r="B57" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="C57" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="D57" s="44">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="74"/>
-      <c r="B14" s="43" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="73"/>
+      <c r="B58" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="D58" s="44">
         <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="74"/>
-      <c r="B15" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="45">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="74" t="s">
-        <v>129</v>
-      </c>
-      <c r="B16" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="74"/>
-      <c r="B17" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="74"/>
-      <c r="B18" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="74"/>
-      <c r="B19" s="44" t="s">
-        <v>171</v>
-      </c>
-      <c r="C19" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="D19" s="46"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="74"/>
-      <c r="B20" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="74" t="s">
-        <v>130</v>
-      </c>
-      <c r="B21" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="74"/>
-      <c r="B22" s="43" t="s">
-        <v>91</v>
-      </c>
-      <c r="C22" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="74"/>
-      <c r="B23" s="43" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="74"/>
-      <c r="B24" s="43" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="74"/>
-      <c r="B25" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="45">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="74"/>
-      <c r="B26" s="43" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="74"/>
-      <c r="B27" s="43" t="s">
-        <v>96</v>
-      </c>
-      <c r="C27" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="74"/>
-      <c r="B28" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="C28" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="74"/>
-      <c r="B29" s="43" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="74"/>
-      <c r="B30" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="C30" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="74"/>
-      <c r="B31" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="D31" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="74" t="s">
-        <v>131</v>
-      </c>
-      <c r="B32" s="43" t="s">
-        <v>101</v>
-      </c>
-      <c r="C32" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="45">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="74"/>
-      <c r="B33" s="43" t="s">
-        <v>102</v>
-      </c>
-      <c r="C33" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="45">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="74"/>
-      <c r="B34" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="C34" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="45">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="74"/>
-      <c r="B35" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="C35" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="45">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="74"/>
-      <c r="B36" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="C36" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="D36" s="45">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="74"/>
-      <c r="B37" s="43" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="D37" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="74"/>
-      <c r="B38" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="C38" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="D38" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="74"/>
-      <c r="B39" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="C39" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="74" t="s">
-        <v>132</v>
-      </c>
-      <c r="B40" s="43" t="s">
-        <v>109</v>
-      </c>
-      <c r="C40" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="D40" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="74"/>
-      <c r="B41" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="C41" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="74"/>
-      <c r="B42" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="C42" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="D42" s="45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="74"/>
-      <c r="B43" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="C43" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="D43" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="74"/>
-      <c r="B44" s="43" t="s">
-        <v>113</v>
-      </c>
-      <c r="C44" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="D44" s="45">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="74"/>
-      <c r="B45" s="43" t="s">
-        <v>114</v>
-      </c>
-      <c r="C45" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="D45" s="45">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="74"/>
-      <c r="B46" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="C46" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="D46" s="45">
-        <v>1.1200000000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="74"/>
-      <c r="B47" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="C47" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="D47" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="74" t="s">
-        <v>133</v>
-      </c>
-      <c r="B48" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="C48" s="47" t="s">
-        <v>66</v>
-      </c>
-      <c r="D48" s="45">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="74"/>
-      <c r="B49" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="C49" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="D49" s="45">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="74"/>
-      <c r="B50" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="C50" s="47" t="s">
-        <v>68</v>
-      </c>
-      <c r="D50" s="45">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="74" t="s">
-        <v>134</v>
-      </c>
-      <c r="B51" s="43" t="s">
-        <v>120</v>
-      </c>
-      <c r="C51" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="D51" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="74"/>
-      <c r="B52" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="C52" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="D52" s="45">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="74"/>
-      <c r="B53" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="C53" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="D53" s="45">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="74"/>
-      <c r="B54" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="C54" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="D54" s="45">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="74"/>
-      <c r="B55" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="C55" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="D55" s="45">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="74"/>
-      <c r="B56" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="C56" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="D56" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="74" t="s">
-        <v>135</v>
-      </c>
-      <c r="B57" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="C57" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="D57" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="74"/>
-      <c r="B58" s="43" t="s">
-        <v>127</v>
-      </c>
-      <c r="C58" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="D58" s="45">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -13653,17 +14289,17 @@
     <mergeCell ref="D2:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:D58">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>$D$4&lt;&gt;FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:D4">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$D$4=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$D$4=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13695,8 +14331,8 @@
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.5703125" style="15" customWidth="1"/>
-    <col min="2" max="2" width="54.42578125" style="43" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.42578125" style="42" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="46" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" style="15" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="15" hidden="1"/>
   </cols>
@@ -13705,33 +14341,33 @@
       <c r="A1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="60"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="75" t="str">
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="74" t="str">
         <f>IF($D$4="","Cannot be empty, please enter FALSE","")</f>
         <v/>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="60"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="75"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="74"/>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="B4" s="43" t="s">
-        <v>245</v>
-      </c>
-      <c r="C4" s="47" t="s">
+      <c r="B4" s="42" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="46" t="s">
         <v>189</v>
       </c>
       <c r="D4" s="17" t="s">
@@ -13739,126 +14375,126 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="73" t="s">
         <v>137</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="46" t="s">
         <v>188</v>
       </c>
-      <c r="D5" s="50">
+      <c r="D5" s="49">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="74"/>
-      <c r="B6" s="43" t="s">
+      <c r="A6" s="73"/>
+      <c r="B6" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="74"/>
-      <c r="B7" s="43" t="s">
+      <c r="A7" s="73"/>
+      <c r="B7" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="D7" s="50">
+      <c r="D7" s="49">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="74"/>
-      <c r="B8" s="43" t="s">
+      <c r="A8" s="73"/>
+      <c r="B8" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="D8" s="50">
+      <c r="D8" s="49">
         <v>500</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="74"/>
-      <c r="B9" s="43" t="s">
+      <c r="A9" s="73"/>
+      <c r="B9" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="46" t="s">
         <v>142</v>
       </c>
-      <c r="D9" s="50">
+      <c r="D9" s="49">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="74"/>
-      <c r="B10" s="43" t="s">
+      <c r="A10" s="73"/>
+      <c r="B10" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="D10" s="45">
+      <c r="D10" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="s">
+      <c r="A11" s="73" t="s">
         <v>138</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="D11" s="45">
+      <c r="D11" s="44">
         <v>0.01</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="74"/>
-      <c r="B12" s="43" t="s">
+      <c r="A12" s="73"/>
+      <c r="B12" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="D12" s="45">
+      <c r="D12" s="44">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="74"/>
-      <c r="B13" s="43" t="s">
+      <c r="A13" s="73"/>
+      <c r="B13" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="D13" s="45">
+      <c r="D13" s="44">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="74"/>
-      <c r="B14" s="43" t="s">
+      <c r="A14" s="73"/>
+      <c r="B14" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="D14" s="45">
+      <c r="D14" s="44">
         <v>0</v>
       </c>
     </row>
@@ -13872,22 +14508,22 @@
     <mergeCell ref="A2:C3"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:D4">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$D$4=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$D$4=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:D14">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>$D$4&lt;&gt;FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>AND($B$13,$D$9&gt;=$D$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13916,6 +14552,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -14067,15 +14712,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
   <ds:schemaRefs>
@@ -14093,6 +14729,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14108,12 +14752,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>